<commit_message>
fix: condition files, psychopy, xmls and fake data
</commit_message>
<xml_diff>
--- a/conditions/mTBIconditions2.xlsx
+++ b/conditions/mTBIconditions2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="392" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="445" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t>arrow</t>
   </si>
@@ -28,25 +28,19 @@
     <t>q_or_r</t>
   </si>
   <si>
-    <t>opacity</t>
-  </si>
-  <si>
     <t>down</t>
   </si>
   <si>
-    <t>down.jpg</t>
-  </si>
-  <si>
-    <t>Question?</t>
+    <t>images/down.jpg</t>
+  </si>
+  <si>
+    <t>Rate your ability to control your brain</t>
   </si>
   <si>
     <t>up</t>
   </si>
   <si>
-    <t>up.jpg</t>
-  </si>
-  <si>
-    <t>Rest</t>
+    <t>images/up.jpg</t>
   </si>
 </sst>
 </file>
@@ -121,8 +115,9 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -140,14 +135,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B16" activeCellId="0" pane="topLeft" sqref="B16"/>
+      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.321568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -160,92 +158,71 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -271,7 +248,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -296,7 +273,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>